<commit_message>
Deploy to GitHub pages
</commit_message>
<xml_diff>
--- a/StructureDefinition-area-type.xlsx
+++ b/StructureDefinition-area-type.xlsx
@@ -206,7 +206,7 @@
     <t>The definition may point directly to a computable or human-readable definition of the extensibility codes, or it may be a logical URI as declared in some other specification. The definition SHALL be a URI for the Structure Definition defining the extension.</t>
   </si>
   <si>
-    <t>http://example.org/StructureDefinition/area-type</t>
+    <t>https://jembi.github.io/commcare-vaccine-ig//StructureDefinition/area-type</t>
   </si>
   <si>
     <t>N/A</t>
@@ -242,7 +242,7 @@
     <t>required</t>
   </si>
   <si>
-    <t>http://example.org/ValueSet/area-type-vs</t>
+    <t>https://jembi.github.io/commcare-vaccine-ig//ValueSet/area-type-vs</t>
   </si>
 </sst>
 </file>
@@ -424,7 +424,7 @@
     <col min="22" max="22" width="19.03125" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="18.85546875" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="21.5703125" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="39.21484375" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="63.3671875" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="6.34765625" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="22.71484375" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="42.03125" customWidth="true" bestFit="true"/>

</xml_diff>